<commit_message>
Finishes Chapter3_5, except for calculations needed on blaze optimal incidence.
</commit_message>
<xml_diff>
--- a/data/Extended/OptimalIncidenceGlobalRect/ProblemSetup.xlsx
+++ b/data/Extended/OptimalIncidenceGlobalRect/ProblemSetup.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21405"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="6940" yWindow="1100" windowWidth="25040" windowHeight="17820" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="3760" yWindow="0" windowWidth="25040" windowHeight="17480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,9 +21,6 @@
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
-  <si>
-    <t>90 procs</t>
-  </si>
   <si>
     <t>Height:</t>
   </si>
@@ -53,6 +50,9 @@
   </si>
   <si>
     <t>Results:</t>
+  </si>
+  <si>
+    <t>139 procs</t>
   </si>
 </sst>
 </file>
@@ -458,10 +458,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H151"/>
+  <dimension ref="A1:H141"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -471,36 +471,36 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B1" t="s">
         <v>5</v>
       </c>
       <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" t="s">
         <v>6</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="H1" t="s">
+    </row>
+    <row r="2" spans="1:8">
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" t="s">
-        <v>3</v>
-      </c>
-      <c r="H2" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -508,7 +508,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="D3">
-        <v>74</v>
+        <v>74.999999999999901</v>
       </c>
       <c r="F3">
         <v>1.2E-2</v>
@@ -522,7 +522,7 @@
         <v>6.0000000000000001E-3</v>
       </c>
       <c r="D4">
-        <v>74.099999999999994</v>
+        <v>75.099999999999895</v>
       </c>
       <c r="F4">
         <v>1.15E-2</v>
@@ -536,7 +536,7 @@
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="D5">
-        <v>74.2</v>
+        <v>75.199999999999903</v>
       </c>
       <c r="F5">
         <v>1.0999999999999999E-2</v>
@@ -550,7 +550,7 @@
         <v>0.01</v>
       </c>
       <c r="D6">
-        <v>74.3</v>
+        <v>75.299999999999898</v>
       </c>
       <c r="F6">
         <v>1.0500000000000001E-2</v>
@@ -564,7 +564,7 @@
         <v>1.2E-2</v>
       </c>
       <c r="D7">
-        <v>74.400000000000006</v>
+        <v>75.399999999999906</v>
       </c>
       <c r="F7">
         <v>0.01</v>
@@ -578,7 +578,7 @@
         <v>1.4E-2</v>
       </c>
       <c r="D8">
-        <v>74.5</v>
+        <v>75.499999999999901</v>
       </c>
       <c r="F8">
         <v>9.4999999999999998E-3</v>
@@ -592,7 +592,7 @@
         <v>1.6E-2</v>
       </c>
       <c r="D9">
-        <v>74.599999999999994</v>
+        <v>75.599999999999895</v>
       </c>
       <c r="F9">
         <v>8.9999999999999993E-3</v>
@@ -606,7 +606,7 @@
         <v>1.7999999999999999E-2</v>
       </c>
       <c r="D10">
-        <v>74.7</v>
+        <v>75.699999999999903</v>
       </c>
       <c r="F10">
         <v>8.5000000000000006E-3</v>
@@ -620,7 +620,7 @@
         <v>0.02</v>
       </c>
       <c r="D11">
-        <v>74.8</v>
+        <v>75.799999999999898</v>
       </c>
       <c r="F11">
         <v>8.0000000000000002E-3</v>
@@ -634,7 +634,7 @@
         <v>2.1999999999999999E-2</v>
       </c>
       <c r="D12">
-        <v>74.899999999999906</v>
+        <v>75.899999999999906</v>
       </c>
       <c r="F12">
         <v>7.4999999999999997E-3</v>
@@ -648,7 +648,7 @@
         <v>2.4E-2</v>
       </c>
       <c r="D13">
-        <v>74.999999999999901</v>
+        <v>75.999999999999901</v>
       </c>
       <c r="F13">
         <v>7.0000000000000001E-3</v>
@@ -662,7 +662,7 @@
         <v>2.5999999999999999E-2</v>
       </c>
       <c r="D14">
-        <v>75.099999999999895</v>
+        <v>76.099999999999895</v>
       </c>
       <c r="F14">
         <v>6.4999999999999997E-3</v>
@@ -673,7 +673,7 @@
         <v>2.8000000000000001E-2</v>
       </c>
       <c r="D15">
-        <v>75.199999999999903</v>
+        <v>76.199999999999903</v>
       </c>
       <c r="F15">
         <v>5.9999999999999897E-3</v>
@@ -684,7 +684,7 @@
         <v>0.03</v>
       </c>
       <c r="D16">
-        <v>75.299999999999898</v>
+        <v>76.299999999999898</v>
       </c>
       <c r="F16">
         <v>5.4999999999999901E-3</v>
@@ -695,7 +695,7 @@
         <v>3.2000000000000001E-2</v>
       </c>
       <c r="D17">
-        <v>75.399999999999906</v>
+        <v>76.399999999999906</v>
       </c>
       <c r="F17">
         <v>4.9999999999999897E-3</v>
@@ -706,7 +706,7 @@
         <v>3.4000000000000002E-2</v>
       </c>
       <c r="D18">
-        <v>75.499999999999901</v>
+        <v>76.499999999999901</v>
       </c>
       <c r="F18">
         <v>4.4999999999999901E-3</v>
@@ -717,7 +717,7 @@
         <v>3.5999999999999997E-2</v>
       </c>
       <c r="D19">
-        <v>75.599999999999895</v>
+        <v>76.599999999999895</v>
       </c>
       <c r="F19">
         <v>3.9999999999999897E-3</v>
@@ -728,7 +728,7 @@
         <v>3.7999999999999999E-2</v>
       </c>
       <c r="D20">
-        <v>75.699999999999903</v>
+        <v>76.699999999999804</v>
       </c>
       <c r="F20">
         <v>3.4999999999999901E-3</v>
@@ -739,7 +739,7 @@
         <v>0.04</v>
       </c>
       <c r="D21">
-        <v>75.799999999999898</v>
+        <v>76.799999999999798</v>
       </c>
       <c r="F21">
         <v>2.9999999999999901E-3</v>
@@ -750,7 +750,7 @@
         <v>4.2000000000000003E-2</v>
       </c>
       <c r="D22">
-        <v>75.899999999999906</v>
+        <v>76.899999999999807</v>
       </c>
       <c r="F22">
         <v>2.4999999999999901E-3</v>
@@ -761,7 +761,7 @@
         <v>4.3999999999999997E-2</v>
       </c>
       <c r="D23">
-        <v>75.999999999999901</v>
+        <v>76.999999999999801</v>
       </c>
       <c r="F23">
         <v>2E-3</v>
@@ -772,7 +772,7 @@
         <v>4.5999999999999999E-2</v>
       </c>
       <c r="D24">
-        <v>76.099999999999895</v>
+        <v>77.099999999999795</v>
       </c>
       <c r="F24">
         <v>1.5E-3</v>
@@ -783,7 +783,7 @@
         <v>4.8000000000000001E-2</v>
       </c>
       <c r="D25">
-        <v>76.199999999999903</v>
+        <v>77.199999999999804</v>
       </c>
       <c r="F25">
         <v>1E-3</v>
@@ -794,7 +794,7 @@
         <v>0.05</v>
       </c>
       <c r="D26">
-        <v>76.299999999999898</v>
+        <v>77.299999999999798</v>
       </c>
     </row>
     <row r="27" spans="2:6">
@@ -802,7 +802,7 @@
         <v>5.1999999999999998E-2</v>
       </c>
       <c r="D27">
-        <v>76.399999999999906</v>
+        <v>77.399999999999807</v>
       </c>
     </row>
     <row r="28" spans="2:6">
@@ -810,7 +810,7 @@
         <v>5.3999999999999999E-2</v>
       </c>
       <c r="D28">
-        <v>76.499999999999901</v>
+        <v>77.499999999999801</v>
       </c>
     </row>
     <row r="29" spans="2:6">
@@ -818,7 +818,7 @@
         <v>5.6000000000000001E-2</v>
       </c>
       <c r="D29">
-        <v>76.599999999999895</v>
+        <v>77.599999999999795</v>
       </c>
     </row>
     <row r="30" spans="2:6">
@@ -826,7 +826,7 @@
         <v>5.8000000000000003E-2</v>
       </c>
       <c r="D30">
-        <v>76.699999999999804</v>
+        <v>77.699999999999804</v>
       </c>
     </row>
     <row r="31" spans="2:6">
@@ -834,7 +834,7 @@
         <v>0.06</v>
       </c>
       <c r="D31">
-        <v>76.799999999999798</v>
+        <v>77.799999999999798</v>
       </c>
     </row>
     <row r="32" spans="2:6">
@@ -842,7 +842,7 @@
         <v>6.2E-2</v>
       </c>
       <c r="D32">
-        <v>76.899999999999807</v>
+        <v>77.899999999999807</v>
       </c>
     </row>
     <row r="33" spans="2:4">
@@ -850,7 +850,7 @@
         <v>6.4000000000000001E-2</v>
       </c>
       <c r="D33">
-        <v>76.999999999999801</v>
+        <v>77.999999999999801</v>
       </c>
     </row>
     <row r="34" spans="2:4">
@@ -858,7 +858,7 @@
         <v>6.6000000000000003E-2</v>
       </c>
       <c r="D34">
-        <v>77.099999999999795</v>
+        <v>78.099999999999795</v>
       </c>
     </row>
     <row r="35" spans="2:4">
@@ -866,7 +866,7 @@
         <v>6.8000000000000005E-2</v>
       </c>
       <c r="D35">
-        <v>77.199999999999804</v>
+        <v>78.199999999999804</v>
       </c>
     </row>
     <row r="36" spans="2:4">
@@ -874,7 +874,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="D36">
-        <v>77.299999999999798</v>
+        <v>78.299999999999798</v>
       </c>
     </row>
     <row r="37" spans="2:4">
@@ -882,7 +882,7 @@
         <v>7.1999999999999995E-2</v>
       </c>
       <c r="D37">
-        <v>77.399999999999807</v>
+        <v>78.399999999999693</v>
       </c>
     </row>
     <row r="38" spans="2:4">
@@ -890,7 +890,7 @@
         <v>7.3999999999999996E-2</v>
       </c>
       <c r="D38">
-        <v>77.499999999999801</v>
+        <v>78.499999999999702</v>
       </c>
     </row>
     <row r="39" spans="2:4">
@@ -898,7 +898,7 @@
         <v>7.5999999999999998E-2</v>
       </c>
       <c r="D39">
-        <v>77.599999999999795</v>
+        <v>78.599999999999696</v>
       </c>
     </row>
     <row r="40" spans="2:4">
@@ -906,7 +906,7 @@
         <v>7.8E-2</v>
       </c>
       <c r="D40">
-        <v>77.699999999999804</v>
+        <v>78.699999999999704</v>
       </c>
     </row>
     <row r="41" spans="2:4">
@@ -914,7 +914,7 @@
         <v>0.08</v>
       </c>
       <c r="D41">
-        <v>77.799999999999798</v>
+        <v>78.799999999999699</v>
       </c>
     </row>
     <row r="42" spans="2:4">
@@ -922,7 +922,7 @@
         <v>8.2000000000000003E-2</v>
       </c>
       <c r="D42">
-        <v>77.899999999999807</v>
+        <v>78.899999999999693</v>
       </c>
     </row>
     <row r="43" spans="2:4">
@@ -930,7 +930,7 @@
         <v>8.4000000000000005E-2</v>
       </c>
       <c r="D43">
-        <v>77.999999999999801</v>
+        <v>78.999999999999702</v>
       </c>
     </row>
     <row r="44" spans="2:4">
@@ -938,7 +938,7 @@
         <v>8.5999999999999993E-2</v>
       </c>
       <c r="D44">
-        <v>78.099999999999795</v>
+        <v>79.099999999999696</v>
       </c>
     </row>
     <row r="45" spans="2:4">
@@ -946,7 +946,7 @@
         <v>8.7999999999999995E-2</v>
       </c>
       <c r="D45">
-        <v>78.199999999999804</v>
+        <v>79.199999999999704</v>
       </c>
     </row>
     <row r="46" spans="2:4">
@@ -954,7 +954,7 @@
         <v>0.09</v>
       </c>
       <c r="D46">
-        <v>78.299999999999798</v>
+        <v>79.299999999999699</v>
       </c>
     </row>
     <row r="47" spans="2:4">
@@ -962,7 +962,7 @@
         <v>9.1999999999999998E-2</v>
       </c>
       <c r="D47">
-        <v>78.399999999999693</v>
+        <v>79.399999999999693</v>
       </c>
     </row>
     <row r="48" spans="2:4">
@@ -970,7 +970,7 @@
         <v>9.4E-2</v>
       </c>
       <c r="D48">
-        <v>78.499999999999702</v>
+        <v>79.499999999999702</v>
       </c>
     </row>
     <row r="49" spans="2:4">
@@ -978,7 +978,7 @@
         <v>9.6000000000000002E-2</v>
       </c>
       <c r="D49">
-        <v>78.599999999999696</v>
+        <v>79.599999999999696</v>
       </c>
     </row>
     <row r="50" spans="2:4">
@@ -986,7 +986,7 @@
         <v>9.8000000000000004E-2</v>
       </c>
       <c r="D50">
-        <v>78.699999999999704</v>
+        <v>79.699999999999704</v>
       </c>
     </row>
     <row r="51" spans="2:4">
@@ -994,7 +994,7 @@
         <v>0.1</v>
       </c>
       <c r="D51">
-        <v>78.799999999999699</v>
+        <v>79.799999999999699</v>
       </c>
     </row>
     <row r="52" spans="2:4">
@@ -1002,7 +1002,7 @@
         <v>0.10199999999999999</v>
       </c>
       <c r="D52">
-        <v>78.899999999999693</v>
+        <v>79.899999999999693</v>
       </c>
     </row>
     <row r="53" spans="2:4">
@@ -1010,7 +1010,7 @@
         <v>0.104</v>
       </c>
       <c r="D53">
-        <v>78.999999999999702</v>
+        <v>79.999999999999702</v>
       </c>
     </row>
     <row r="54" spans="2:4">
@@ -1018,7 +1018,7 @@
         <v>0.106</v>
       </c>
       <c r="D54">
-        <v>79.099999999999696</v>
+        <v>80.099999999999696</v>
       </c>
     </row>
     <row r="55" spans="2:4">
@@ -1026,7 +1026,7 @@
         <v>0.108</v>
       </c>
       <c r="D55">
-        <v>79.199999999999704</v>
+        <v>80.199999999999605</v>
       </c>
     </row>
     <row r="56" spans="2:4">
@@ -1034,7 +1034,7 @@
         <v>0.11</v>
       </c>
       <c r="D56">
-        <v>79.299999999999699</v>
+        <v>80.299999999999599</v>
       </c>
     </row>
     <row r="57" spans="2:4">
@@ -1042,7 +1042,7 @@
         <v>0.112</v>
       </c>
       <c r="D57">
-        <v>79.399999999999693</v>
+        <v>80.399999999999594</v>
       </c>
     </row>
     <row r="58" spans="2:4">
@@ -1050,7 +1050,7 @@
         <v>0.114</v>
       </c>
       <c r="D58">
-        <v>79.499999999999702</v>
+        <v>80.499999999999602</v>
       </c>
     </row>
     <row r="59" spans="2:4">
@@ -1058,7 +1058,7 @@
         <v>0.11600000000000001</v>
       </c>
       <c r="D59">
-        <v>79.599999999999696</v>
+        <v>80.599999999999596</v>
       </c>
     </row>
     <row r="60" spans="2:4">
@@ -1066,7 +1066,7 @@
         <v>0.11799999999999999</v>
       </c>
       <c r="D60">
-        <v>79.699999999999704</v>
+        <v>80.699999999999605</v>
       </c>
     </row>
     <row r="61" spans="2:4">
@@ -1074,7 +1074,7 @@
         <v>0.12</v>
       </c>
       <c r="D61">
-        <v>79.799999999999699</v>
+        <v>80.799999999999599</v>
       </c>
     </row>
     <row r="62" spans="2:4">
@@ -1082,7 +1082,7 @@
         <v>0.122</v>
       </c>
       <c r="D62">
-        <v>79.899999999999693</v>
+        <v>80.899999999999594</v>
       </c>
     </row>
     <row r="63" spans="2:4">
@@ -1090,7 +1090,7 @@
         <v>0.124</v>
       </c>
       <c r="D63">
-        <v>79.999999999999702</v>
+        <v>80.999999999999602</v>
       </c>
     </row>
     <row r="64" spans="2:4">
@@ -1098,7 +1098,7 @@
         <v>0.126</v>
       </c>
       <c r="D64">
-        <v>80.099999999999696</v>
+        <v>81.099999999999596</v>
       </c>
     </row>
     <row r="65" spans="2:4">
@@ -1106,7 +1106,7 @@
         <v>0.128</v>
       </c>
       <c r="D65">
-        <v>80.199999999999605</v>
+        <v>81.199999999999605</v>
       </c>
     </row>
     <row r="66" spans="2:4">
@@ -1114,7 +1114,7 @@
         <v>0.13</v>
       </c>
       <c r="D66">
-        <v>80.299999999999599</v>
+        <v>81.299999999999599</v>
       </c>
     </row>
     <row r="67" spans="2:4">
@@ -1122,7 +1122,7 @@
         <v>0.13200000000000001</v>
       </c>
       <c r="D67">
-        <v>80.399999999999594</v>
+        <v>81.399999999999594</v>
       </c>
     </row>
     <row r="68" spans="2:4">
@@ -1130,7 +1130,7 @@
         <v>0.13400000000000001</v>
       </c>
       <c r="D68">
-        <v>80.499999999999602</v>
+        <v>81.499999999999602</v>
       </c>
     </row>
     <row r="69" spans="2:4">
@@ -1138,7 +1138,7 @@
         <v>0.13600000000000001</v>
       </c>
       <c r="D69">
-        <v>80.599999999999596</v>
+        <v>81.599999999999596</v>
       </c>
     </row>
     <row r="70" spans="2:4">
@@ -1146,7 +1146,7 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="D70">
-        <v>80.699999999999605</v>
+        <v>81.699999999999605</v>
       </c>
     </row>
     <row r="71" spans="2:4">
@@ -1154,7 +1154,7 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="D71">
-        <v>80.799999999999599</v>
+        <v>81.799999999999599</v>
       </c>
     </row>
     <row r="72" spans="2:4">
@@ -1162,7 +1162,7 @@
         <v>0.14199999999999999</v>
       </c>
       <c r="D72">
-        <v>80.899999999999594</v>
+        <v>81.899999999999594</v>
       </c>
     </row>
     <row r="73" spans="2:4">
@@ -1170,7 +1170,7 @@
         <v>0.14399999999999999</v>
       </c>
       <c r="D73">
-        <v>80.999999999999602</v>
+        <v>81.999999999999503</v>
       </c>
     </row>
     <row r="74" spans="2:4">
@@ -1178,7 +1178,7 @@
         <v>0.14599999999999999</v>
       </c>
       <c r="D74">
-        <v>81.099999999999596</v>
+        <v>82.099999999999497</v>
       </c>
     </row>
     <row r="75" spans="2:4">
@@ -1186,7 +1186,7 @@
         <v>0.14799999999999999</v>
       </c>
       <c r="D75">
-        <v>81.199999999999605</v>
+        <v>82.199999999999505</v>
       </c>
     </row>
     <row r="76" spans="2:4">
@@ -1194,7 +1194,7 @@
         <v>0.15</v>
       </c>
       <c r="D76">
-        <v>81.299999999999599</v>
+        <v>82.2999999999995</v>
       </c>
     </row>
     <row r="77" spans="2:4">
@@ -1202,7 +1202,7 @@
         <v>0.152</v>
       </c>
       <c r="D77">
-        <v>81.399999999999594</v>
+        <v>82.399999999999494</v>
       </c>
     </row>
     <row r="78" spans="2:4">
@@ -1210,7 +1210,7 @@
         <v>0.154</v>
       </c>
       <c r="D78">
-        <v>81.499999999999602</v>
+        <v>82.499999999999503</v>
       </c>
     </row>
     <row r="79" spans="2:4">
@@ -1218,7 +1218,7 @@
         <v>0.156</v>
       </c>
       <c r="D79">
-        <v>81.599999999999596</v>
+        <v>82.599999999999497</v>
       </c>
     </row>
     <row r="80" spans="2:4">
@@ -1226,7 +1226,7 @@
         <v>0.158</v>
       </c>
       <c r="D80">
-        <v>81.699999999999605</v>
+        <v>82.699999999999505</v>
       </c>
     </row>
     <row r="81" spans="2:4">
@@ -1234,7 +1234,7 @@
         <v>0.16</v>
       </c>
       <c r="D81">
-        <v>81.799999999999599</v>
+        <v>82.7999999999995</v>
       </c>
     </row>
     <row r="82" spans="2:4">
@@ -1242,7 +1242,7 @@
         <v>0.16200000000000001</v>
       </c>
       <c r="D82">
-        <v>81.899999999999594</v>
+        <v>82.899999999999494</v>
       </c>
     </row>
     <row r="83" spans="2:4">
@@ -1250,7 +1250,7 @@
         <v>0.16400000000000001</v>
       </c>
       <c r="D83">
-        <v>81.999999999999503</v>
+        <v>82.999999999999503</v>
       </c>
     </row>
     <row r="84" spans="2:4">
@@ -1258,7 +1258,7 @@
         <v>0.16600000000000001</v>
       </c>
       <c r="D84">
-        <v>82.099999999999497</v>
+        <v>83.099999999999497</v>
       </c>
     </row>
     <row r="85" spans="2:4">
@@ -1266,7 +1266,7 @@
         <v>0.16800000000000001</v>
       </c>
       <c r="D85">
-        <v>82.199999999999505</v>
+        <v>83.199999999999505</v>
       </c>
     </row>
     <row r="86" spans="2:4">
@@ -1274,7 +1274,7 @@
         <v>0.17</v>
       </c>
       <c r="D86">
-        <v>82.2999999999995</v>
+        <v>83.2999999999995</v>
       </c>
     </row>
     <row r="87" spans="2:4">
@@ -1282,7 +1282,7 @@
         <v>0.17199999999999999</v>
       </c>
       <c r="D87">
-        <v>82.399999999999494</v>
+        <v>83.399999999999494</v>
       </c>
     </row>
     <row r="88" spans="2:4">
@@ -1290,7 +1290,7 @@
         <v>0.17399999999999999</v>
       </c>
       <c r="D88">
-        <v>82.499999999999503</v>
+        <v>83.499999999999503</v>
       </c>
     </row>
     <row r="89" spans="2:4">
@@ -1298,7 +1298,7 @@
         <v>0.17599999999999999</v>
       </c>
       <c r="D89">
-        <v>82.599999999999497</v>
+        <v>83.599999999999497</v>
       </c>
     </row>
     <row r="90" spans="2:4">
@@ -1306,7 +1306,7 @@
         <v>0.17799999999999999</v>
       </c>
       <c r="D90">
-        <v>82.699999999999505</v>
+        <v>83.699999999999406</v>
       </c>
     </row>
     <row r="91" spans="2:4">
@@ -1314,306 +1314,256 @@
         <v>0.18</v>
       </c>
       <c r="D91">
-        <v>82.7999999999995</v>
+        <v>83.7999999999994</v>
       </c>
     </row>
     <row r="92" spans="2:4">
       <c r="D92">
-        <v>82.899999999999494</v>
+        <v>83.899999999999395</v>
       </c>
     </row>
     <row r="93" spans="2:4">
       <c r="D93">
-        <v>82.999999999999503</v>
+        <v>83.999999999999403</v>
       </c>
     </row>
     <row r="94" spans="2:4">
       <c r="D94">
-        <v>83.099999999999497</v>
+        <v>84.099999999999397</v>
       </c>
     </row>
     <row r="95" spans="2:4">
       <c r="D95">
-        <v>83.199999999999505</v>
+        <v>84.199999999999406</v>
       </c>
     </row>
     <row r="96" spans="2:4">
       <c r="D96">
-        <v>83.2999999999995</v>
+        <v>84.2999999999994</v>
       </c>
     </row>
     <row r="97" spans="4:4">
       <c r="D97">
-        <v>83.399999999999494</v>
+        <v>84.399999999999395</v>
       </c>
     </row>
     <row r="98" spans="4:4">
       <c r="D98">
-        <v>83.499999999999503</v>
+        <v>84.499999999999403</v>
       </c>
     </row>
     <row r="99" spans="4:4">
       <c r="D99">
-        <v>83.599999999999497</v>
+        <v>84.599999999999397</v>
       </c>
     </row>
     <row r="100" spans="4:4">
       <c r="D100">
-        <v>83.699999999999406</v>
+        <v>84.699999999999406</v>
       </c>
     </row>
     <row r="101" spans="4:4">
       <c r="D101">
-        <v>83.7999999999994</v>
+        <v>84.7999999999994</v>
       </c>
     </row>
     <row r="102" spans="4:4">
       <c r="D102">
-        <v>83.899999999999395</v>
+        <v>84.899999999999395</v>
       </c>
     </row>
     <row r="103" spans="4:4">
       <c r="D103">
-        <v>83.999999999999403</v>
+        <v>84.999999999999403</v>
       </c>
     </row>
     <row r="104" spans="4:4">
       <c r="D104">
-        <v>84.099999999999397</v>
+        <v>85.099999999999397</v>
       </c>
     </row>
     <row r="105" spans="4:4">
       <c r="D105">
-        <v>84.199999999999406</v>
+        <v>85.199999999999406</v>
       </c>
     </row>
     <row r="106" spans="4:4">
       <c r="D106">
-        <v>84.2999999999994</v>
+        <v>85.2999999999994</v>
       </c>
     </row>
     <row r="107" spans="4:4">
       <c r="D107">
-        <v>84.399999999999395</v>
+        <v>85.399999999999395</v>
       </c>
     </row>
     <row r="108" spans="4:4">
       <c r="D108">
-        <v>84.499999999999403</v>
+        <v>85.499999999999304</v>
       </c>
     </row>
     <row r="109" spans="4:4">
       <c r="D109">
-        <v>84.599999999999397</v>
+        <v>85.599999999999298</v>
       </c>
     </row>
     <row r="110" spans="4:4">
       <c r="D110">
-        <v>84.699999999999406</v>
+        <v>85.699999999999307</v>
       </c>
     </row>
     <row r="111" spans="4:4">
       <c r="D111">
-        <v>84.7999999999994</v>
+        <v>85.799999999999301</v>
       </c>
     </row>
     <row r="112" spans="4:4">
       <c r="D112">
-        <v>84.899999999999395</v>
+        <v>85.899999999999295</v>
       </c>
     </row>
     <row r="113" spans="4:4">
       <c r="D113">
-        <v>84.999999999999403</v>
+        <v>85.999999999999304</v>
       </c>
     </row>
     <row r="114" spans="4:4">
       <c r="D114">
-        <v>85.099999999999397</v>
+        <v>86.099999999999298</v>
       </c>
     </row>
     <row r="115" spans="4:4">
       <c r="D115">
-        <v>85.199999999999406</v>
+        <v>86.199999999999307</v>
       </c>
     </row>
     <row r="116" spans="4:4">
       <c r="D116">
-        <v>85.2999999999994</v>
+        <v>86.299999999999301</v>
       </c>
     </row>
     <row r="117" spans="4:4">
       <c r="D117">
-        <v>85.399999999999395</v>
+        <v>86.399999999999295</v>
       </c>
     </row>
     <row r="118" spans="4:4">
       <c r="D118">
-        <v>85.499999999999304</v>
+        <v>86.499999999999304</v>
       </c>
     </row>
     <row r="119" spans="4:4">
       <c r="D119">
-        <v>85.599999999999298</v>
+        <v>86.599999999999298</v>
       </c>
     </row>
     <row r="120" spans="4:4">
       <c r="D120">
-        <v>85.699999999999307</v>
+        <v>86.699999999999307</v>
       </c>
     </row>
     <row r="121" spans="4:4">
       <c r="D121">
-        <v>85.799999999999301</v>
+        <v>86.799999999999301</v>
       </c>
     </row>
     <row r="122" spans="4:4">
       <c r="D122">
-        <v>85.899999999999295</v>
+        <v>86.899999999999295</v>
       </c>
     </row>
     <row r="123" spans="4:4">
       <c r="D123">
-        <v>85.999999999999304</v>
+        <v>86.999999999999304</v>
       </c>
     </row>
     <row r="124" spans="4:4">
       <c r="D124">
-        <v>86.099999999999298</v>
+        <v>87.099999999999298</v>
       </c>
     </row>
     <row r="125" spans="4:4">
       <c r="D125">
-        <v>86.199999999999307</v>
+        <v>87.199999999999207</v>
       </c>
     </row>
     <row r="126" spans="4:4">
       <c r="D126">
-        <v>86.299999999999301</v>
+        <v>87.299999999999201</v>
       </c>
     </row>
     <row r="127" spans="4:4">
       <c r="D127">
-        <v>86.399999999999295</v>
+        <v>87.399999999999196</v>
       </c>
     </row>
     <row r="128" spans="4:4">
       <c r="D128">
-        <v>86.499999999999304</v>
+        <v>87.499999999999204</v>
       </c>
     </row>
     <row r="129" spans="4:4">
       <c r="D129">
-        <v>86.599999999999298</v>
+        <v>87.599999999999199</v>
       </c>
     </row>
     <row r="130" spans="4:4">
       <c r="D130">
-        <v>86.699999999999307</v>
+        <v>87.699999999999207</v>
       </c>
     </row>
     <row r="131" spans="4:4">
       <c r="D131">
-        <v>86.799999999999301</v>
+        <v>87.799999999999201</v>
       </c>
     </row>
     <row r="132" spans="4:4">
       <c r="D132">
-        <v>86.899999999999295</v>
+        <v>87.899999999999196</v>
       </c>
     </row>
     <row r="133" spans="4:4">
       <c r="D133">
-        <v>86.999999999999304</v>
+        <v>87.999999999999204</v>
       </c>
     </row>
     <row r="134" spans="4:4">
       <c r="D134">
-        <v>87.099999999999298</v>
+        <v>88.099999999999199</v>
       </c>
     </row>
     <row r="135" spans="4:4">
       <c r="D135">
-        <v>87.199999999999207</v>
+        <v>88.199999999999207</v>
       </c>
     </row>
     <row r="136" spans="4:4">
       <c r="D136">
-        <v>87.299999999999201</v>
+        <v>88.299999999999201</v>
       </c>
     </row>
     <row r="137" spans="4:4">
       <c r="D137">
-        <v>87.399999999999196</v>
+        <v>88.399999999999196</v>
       </c>
     </row>
     <row r="138" spans="4:4">
       <c r="D138">
-        <v>87.499999999999204</v>
+        <v>88.499999999999204</v>
       </c>
     </row>
     <row r="139" spans="4:4">
       <c r="D139">
-        <v>87.599999999999199</v>
+        <v>88.599999999999199</v>
       </c>
     </row>
     <row r="140" spans="4:4">
       <c r="D140">
-        <v>87.699999999999207</v>
+        <v>88.699999999999207</v>
       </c>
     </row>
     <row r="141" spans="4:4">
       <c r="D141">
-        <v>87.799999999999201</v>
-      </c>
-    </row>
-    <row r="142" spans="4:4">
-      <c r="D142">
-        <v>87.899999999999196</v>
-      </c>
-    </row>
-    <row r="143" spans="4:4">
-      <c r="D143">
-        <v>87.999999999999204</v>
-      </c>
-    </row>
-    <row r="144" spans="4:4">
-      <c r="D144">
-        <v>88.099999999999199</v>
-      </c>
-    </row>
-    <row r="145" spans="4:4">
-      <c r="D145">
-        <v>88.199999999999207</v>
-      </c>
-    </row>
-    <row r="146" spans="4:4">
-      <c r="D146">
-        <v>88.299999999999201</v>
-      </c>
-    </row>
-    <row r="147" spans="4:4">
-      <c r="D147">
-        <v>88.399999999999196</v>
-      </c>
-    </row>
-    <row r="148" spans="4:4">
-      <c r="D148">
-        <v>88.499999999999204</v>
-      </c>
-    </row>
-    <row r="149" spans="4:4">
-      <c r="D149">
-        <v>88.599999999999199</v>
-      </c>
-    </row>
-    <row r="150" spans="4:4">
-      <c r="D150">
-        <v>88.699999999999207</v>
-      </c>
-    </row>
-    <row r="151" spans="4:4">
-      <c r="D151">
         <v>88.799999999999201</v>
       </c>
     </row>
@@ -1632,7 +1582,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -1640,7 +1590,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates fitting of MEG, IMP in chapter5.tex
</commit_message>
<xml_diff>
--- a/data/Extended/OptimalIncidenceGlobalRect/ProblemSetup.xlsx
+++ b/data/Extended/OptimalIncidenceGlobalRect/ProblemSetup.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21405"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3760" yWindow="0" windowWidth="25040" windowHeight="17480" tabRatio="500"/>
+    <workbookView xWindow="2520" yWindow="0" windowWidth="25040" windowHeight="17480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Height:</t>
   </si>
@@ -53,6 +53,12 @@
   </si>
   <si>
     <t>139 procs</t>
+  </si>
+  <si>
+    <t>Blazed:</t>
+  </si>
+  <si>
+    <t>Blaze angles:</t>
   </si>
 </sst>
 </file>
@@ -458,10 +464,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H141"/>
+  <dimension ref="A1:M141"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="D43" sqref="D43:D141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -469,7 +475,7 @@
     <col min="1" max="1" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:13">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -488,8 +494,14 @@
       <c r="H1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:8">
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -503,7 +515,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:13">
       <c r="B3">
         <v>4.0000000000000001E-3</v>
       </c>
@@ -516,8 +528,11 @@
       <c r="H3">
         <v>2.4</v>
       </c>
-    </row>
-    <row r="4" spans="1:8">
+      <c r="M3">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
       <c r="B4">
         <v>6.0000000000000001E-3</v>
       </c>
@@ -530,8 +545,11 @@
       <c r="H4">
         <v>2.2000000000000002</v>
       </c>
-    </row>
-    <row r="5" spans="1:8">
+      <c r="M4">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
       <c r="B5">
         <v>8.0000000000000002E-3</v>
       </c>
@@ -544,8 +562,11 @@
       <c r="H5">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:8">
+      <c r="M5">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
       <c r="B6">
         <v>0.01</v>
       </c>
@@ -558,8 +579,11 @@
       <c r="H6">
         <v>1.8</v>
       </c>
-    </row>
-    <row r="7" spans="1:8">
+      <c r="M6">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
       <c r="B7">
         <v>1.2E-2</v>
       </c>
@@ -572,8 +596,11 @@
       <c r="H7">
         <v>1.6</v>
       </c>
-    </row>
-    <row r="8" spans="1:8">
+      <c r="M7">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
       <c r="B8">
         <v>1.4E-2</v>
       </c>
@@ -586,8 +613,11 @@
       <c r="H8">
         <v>1.4</v>
       </c>
-    </row>
-    <row r="9" spans="1:8">
+      <c r="M8">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
       <c r="B9">
         <v>1.6E-2</v>
       </c>
@@ -600,8 +630,11 @@
       <c r="H9">
         <v>1.2</v>
       </c>
-    </row>
-    <row r="10" spans="1:8">
+      <c r="M9">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
       <c r="B10">
         <v>1.7999999999999999E-2</v>
       </c>
@@ -614,8 +647,11 @@
       <c r="H10">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:8">
+      <c r="M10">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
       <c r="B11">
         <v>0.02</v>
       </c>
@@ -628,8 +664,11 @@
       <c r="H11">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="12" spans="1:8">
+      <c r="M11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
       <c r="B12">
         <v>2.1999999999999999E-2</v>
       </c>
@@ -642,8 +681,11 @@
       <c r="H12">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="13" spans="1:8">
+      <c r="M12">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
       <c r="B13">
         <v>2.4E-2</v>
       </c>
@@ -656,8 +698,11 @@
       <c r="H13">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="14" spans="1:8">
+      <c r="M13">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
       <c r="B14">
         <v>2.5999999999999999E-2</v>
       </c>
@@ -667,8 +712,11 @@
       <c r="F14">
         <v>6.4999999999999997E-3</v>
       </c>
-    </row>
-    <row r="15" spans="1:8">
+      <c r="M14">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
       <c r="B15">
         <v>2.8000000000000001E-2</v>
       </c>
@@ -678,8 +726,11 @@
       <c r="F15">
         <v>5.9999999999999897E-3</v>
       </c>
-    </row>
-    <row r="16" spans="1:8">
+      <c r="M15">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
       <c r="B16">
         <v>0.03</v>
       </c>
@@ -689,8 +740,11 @@
       <c r="F16">
         <v>5.4999999999999901E-3</v>
       </c>
-    </row>
-    <row r="17" spans="2:6">
+      <c r="M16">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="17" spans="2:13">
       <c r="B17">
         <v>3.2000000000000001E-2</v>
       </c>
@@ -700,8 +754,11 @@
       <c r="F17">
         <v>4.9999999999999897E-3</v>
       </c>
-    </row>
-    <row r="18" spans="2:6">
+      <c r="M17">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="18" spans="2:13">
       <c r="B18">
         <v>3.4000000000000002E-2</v>
       </c>
@@ -711,8 +768,11 @@
       <c r="F18">
         <v>4.4999999999999901E-3</v>
       </c>
-    </row>
-    <row r="19" spans="2:6">
+      <c r="M18">
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="19" spans="2:13">
       <c r="B19">
         <v>3.5999999999999997E-2</v>
       </c>
@@ -722,8 +782,11 @@
       <c r="F19">
         <v>3.9999999999999897E-3</v>
       </c>
-    </row>
-    <row r="20" spans="2:6">
+      <c r="M19">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="20" spans="2:13">
       <c r="B20">
         <v>3.7999999999999999E-2</v>
       </c>
@@ -733,8 +796,11 @@
       <c r="F20">
         <v>3.4999999999999901E-3</v>
       </c>
-    </row>
-    <row r="21" spans="2:6">
+      <c r="M20">
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="21" spans="2:13">
       <c r="B21">
         <v>0.04</v>
       </c>
@@ -744,8 +810,11 @@
       <c r="F21">
         <v>2.9999999999999901E-3</v>
       </c>
-    </row>
-    <row r="22" spans="2:6">
+      <c r="M21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="2:13">
       <c r="B22">
         <v>4.2000000000000003E-2</v>
       </c>
@@ -755,8 +824,11 @@
       <c r="F22">
         <v>2.4999999999999901E-3</v>
       </c>
-    </row>
-    <row r="23" spans="2:6">
+      <c r="M22">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="23" spans="2:13">
       <c r="B23">
         <v>4.3999999999999997E-2</v>
       </c>
@@ -766,8 +838,11 @@
       <c r="F23">
         <v>2E-3</v>
       </c>
-    </row>
-    <row r="24" spans="2:6">
+      <c r="M23">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="24" spans="2:13">
       <c r="B24">
         <v>4.5999999999999999E-2</v>
       </c>
@@ -777,8 +852,11 @@
       <c r="F24">
         <v>1.5E-3</v>
       </c>
-    </row>
-    <row r="25" spans="2:6">
+      <c r="M24">
+        <v>2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="25" spans="2:13">
       <c r="B25">
         <v>4.8000000000000001E-2</v>
       </c>
@@ -788,216 +866,297 @@
       <c r="F25">
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="26" spans="2:6">
+      <c r="M25">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="26" spans="2:13">
       <c r="B26">
         <v>0.05</v>
       </c>
       <c r="D26">
         <v>77.299999999999798</v>
       </c>
-    </row>
-    <row r="27" spans="2:6">
+      <c r="M26">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="27" spans="2:13">
       <c r="B27">
         <v>5.1999999999999998E-2</v>
       </c>
       <c r="D27">
         <v>77.399999999999807</v>
       </c>
-    </row>
-    <row r="28" spans="2:6">
+      <c r="M27">
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="28" spans="2:13">
       <c r="B28">
         <v>5.3999999999999999E-2</v>
       </c>
       <c r="D28">
         <v>77.499999999999801</v>
       </c>
-    </row>
-    <row r="29" spans="2:6">
+      <c r="M28">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="29" spans="2:13">
       <c r="B29">
         <v>5.6000000000000001E-2</v>
       </c>
       <c r="D29">
         <v>77.599999999999795</v>
       </c>
-    </row>
-    <row r="30" spans="2:6">
+      <c r="M29">
+        <v>2.8</v>
+      </c>
+    </row>
+    <row r="30" spans="2:13">
       <c r="B30">
         <v>5.8000000000000003E-2</v>
       </c>
       <c r="D30">
         <v>77.699999999999804</v>
       </c>
-    </row>
-    <row r="31" spans="2:6">
+      <c r="M30">
+        <v>2.9</v>
+      </c>
+    </row>
+    <row r="31" spans="2:13">
       <c r="B31">
         <v>0.06</v>
       </c>
       <c r="D31">
         <v>77.799999999999798</v>
       </c>
-    </row>
-    <row r="32" spans="2:6">
+      <c r="M31">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="2:13">
       <c r="B32">
         <v>6.2E-2</v>
       </c>
       <c r="D32">
         <v>77.899999999999807</v>
       </c>
-    </row>
-    <row r="33" spans="2:4">
+      <c r="M32">
+        <v>3.1</v>
+      </c>
+    </row>
+    <row r="33" spans="2:13">
       <c r="B33">
         <v>6.4000000000000001E-2</v>
       </c>
       <c r="D33">
         <v>77.999999999999801</v>
       </c>
-    </row>
-    <row r="34" spans="2:4">
+      <c r="M33">
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="34" spans="2:13">
       <c r="B34">
         <v>6.6000000000000003E-2</v>
       </c>
       <c r="D34">
         <v>78.099999999999795</v>
       </c>
-    </row>
-    <row r="35" spans="2:4">
+      <c r="M34">
+        <v>3.3</v>
+      </c>
+    </row>
+    <row r="35" spans="2:13">
       <c r="B35">
         <v>6.8000000000000005E-2</v>
       </c>
       <c r="D35">
         <v>78.199999999999804</v>
       </c>
-    </row>
-    <row r="36" spans="2:4">
+      <c r="M35">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="36" spans="2:13">
       <c r="B36">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="D36">
         <v>78.299999999999798</v>
       </c>
-    </row>
-    <row r="37" spans="2:4">
+      <c r="M36">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="37" spans="2:13">
       <c r="B37">
         <v>7.1999999999999995E-2</v>
       </c>
       <c r="D37">
         <v>78.399999999999693</v>
       </c>
-    </row>
-    <row r="38" spans="2:4">
+      <c r="M37">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="38" spans="2:13">
       <c r="B38">
         <v>7.3999999999999996E-2</v>
       </c>
       <c r="D38">
         <v>78.499999999999702</v>
       </c>
-    </row>
-    <row r="39" spans="2:4">
+      <c r="M38">
+        <v>3.7</v>
+      </c>
+    </row>
+    <row r="39" spans="2:13">
       <c r="B39">
         <v>7.5999999999999998E-2</v>
       </c>
       <c r="D39">
         <v>78.599999999999696</v>
       </c>
-    </row>
-    <row r="40" spans="2:4">
+      <c r="M39">
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="40" spans="2:13">
       <c r="B40">
         <v>7.8E-2</v>
       </c>
       <c r="D40">
         <v>78.699999999999704</v>
       </c>
-    </row>
-    <row r="41" spans="2:4">
+      <c r="M40">
+        <v>3.9</v>
+      </c>
+    </row>
+    <row r="41" spans="2:13">
       <c r="B41">
         <v>0.08</v>
       </c>
       <c r="D41">
         <v>78.799999999999699</v>
       </c>
-    </row>
-    <row r="42" spans="2:4">
+      <c r="M41">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="2:13">
       <c r="B42">
         <v>8.2000000000000003E-2</v>
       </c>
       <c r="D42">
         <v>78.899999999999693</v>
       </c>
-    </row>
-    <row r="43" spans="2:4">
+      <c r="M42">
+        <v>4.0999999999999996</v>
+      </c>
+    </row>
+    <row r="43" spans="2:13">
       <c r="B43">
         <v>8.4000000000000005E-2</v>
       </c>
       <c r="D43">
         <v>78.999999999999702</v>
       </c>
-    </row>
-    <row r="44" spans="2:4">
+      <c r="M43">
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="44" spans="2:13">
       <c r="B44">
         <v>8.5999999999999993E-2</v>
       </c>
       <c r="D44">
         <v>79.099999999999696</v>
       </c>
-    </row>
-    <row r="45" spans="2:4">
+      <c r="M44">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="45" spans="2:13">
       <c r="B45">
         <v>8.7999999999999995E-2</v>
       </c>
       <c r="D45">
         <v>79.199999999999704</v>
       </c>
-    </row>
-    <row r="46" spans="2:4">
+      <c r="M45">
+        <v>4.4000000000000004</v>
+      </c>
+    </row>
+    <row r="46" spans="2:13">
       <c r="B46">
         <v>0.09</v>
       </c>
       <c r="D46">
         <v>79.299999999999699</v>
       </c>
-    </row>
-    <row r="47" spans="2:4">
+      <c r="M46">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="47" spans="2:13">
       <c r="B47">
         <v>9.1999999999999998E-2</v>
       </c>
       <c r="D47">
         <v>79.399999999999693</v>
       </c>
-    </row>
-    <row r="48" spans="2:4">
+      <c r="M47">
+        <v>4.5999999999999996</v>
+      </c>
+    </row>
+    <row r="48" spans="2:13">
       <c r="B48">
         <v>9.4E-2</v>
       </c>
       <c r="D48">
         <v>79.499999999999702</v>
       </c>
-    </row>
-    <row r="49" spans="2:4">
+      <c r="M48">
+        <v>4.7</v>
+      </c>
+    </row>
+    <row r="49" spans="2:13">
       <c r="B49">
         <v>9.6000000000000002E-2</v>
       </c>
       <c r="D49">
         <v>79.599999999999696</v>
       </c>
-    </row>
-    <row r="50" spans="2:4">
+      <c r="M49">
+        <v>4.8</v>
+      </c>
+    </row>
+    <row r="50" spans="2:13">
       <c r="B50">
         <v>9.8000000000000004E-2</v>
       </c>
       <c r="D50">
         <v>79.699999999999704</v>
       </c>
-    </row>
-    <row r="51" spans="2:4">
+      <c r="M50">
+        <v>4.9000000000000004</v>
+      </c>
+    </row>
+    <row r="51" spans="2:13">
       <c r="B51">
         <v>0.1</v>
       </c>
       <c r="D51">
         <v>79.799999999999699</v>
       </c>
-    </row>
-    <row r="52" spans="2:4">
+      <c r="M51">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="52" spans="2:13">
       <c r="B52">
         <v>0.10199999999999999</v>
       </c>
@@ -1005,7 +1164,7 @@
         <v>79.899999999999693</v>
       </c>
     </row>
-    <row r="53" spans="2:4">
+    <row r="53" spans="2:13">
       <c r="B53">
         <v>0.104</v>
       </c>
@@ -1013,7 +1172,7 @@
         <v>79.999999999999702</v>
       </c>
     </row>
-    <row r="54" spans="2:4">
+    <row r="54" spans="2:13">
       <c r="B54">
         <v>0.106</v>
       </c>
@@ -1021,7 +1180,7 @@
         <v>80.099999999999696</v>
       </c>
     </row>
-    <row r="55" spans="2:4">
+    <row r="55" spans="2:13">
       <c r="B55">
         <v>0.108</v>
       </c>
@@ -1029,7 +1188,7 @@
         <v>80.199999999999605</v>
       </c>
     </row>
-    <row r="56" spans="2:4">
+    <row r="56" spans="2:13">
       <c r="B56">
         <v>0.11</v>
       </c>
@@ -1037,7 +1196,7 @@
         <v>80.299999999999599</v>
       </c>
     </row>
-    <row r="57" spans="2:4">
+    <row r="57" spans="2:13">
       <c r="B57">
         <v>0.112</v>
       </c>
@@ -1045,7 +1204,7 @@
         <v>80.399999999999594</v>
       </c>
     </row>
-    <row r="58" spans="2:4">
+    <row r="58" spans="2:13">
       <c r="B58">
         <v>0.114</v>
       </c>
@@ -1053,7 +1212,7 @@
         <v>80.499999999999602</v>
       </c>
     </row>
-    <row r="59" spans="2:4">
+    <row r="59" spans="2:13">
       <c r="B59">
         <v>0.11600000000000001</v>
       </c>
@@ -1061,7 +1220,7 @@
         <v>80.599999999999596</v>
       </c>
     </row>
-    <row r="60" spans="2:4">
+    <row r="60" spans="2:13">
       <c r="B60">
         <v>0.11799999999999999</v>
       </c>
@@ -1069,7 +1228,7 @@
         <v>80.699999999999605</v>
       </c>
     </row>
-    <row r="61" spans="2:4">
+    <row r="61" spans="2:13">
       <c r="B61">
         <v>0.12</v>
       </c>
@@ -1077,7 +1236,7 @@
         <v>80.799999999999599</v>
       </c>
     </row>
-    <row r="62" spans="2:4">
+    <row r="62" spans="2:13">
       <c r="B62">
         <v>0.122</v>
       </c>
@@ -1085,7 +1244,7 @@
         <v>80.899999999999594</v>
       </c>
     </row>
-    <row r="63" spans="2:4">
+    <row r="63" spans="2:13">
       <c r="B63">
         <v>0.124</v>
       </c>
@@ -1093,7 +1252,7 @@
         <v>80.999999999999602</v>
       </c>
     </row>
-    <row r="64" spans="2:4">
+    <row r="64" spans="2:13">
       <c r="B64">
         <v>0.126</v>
       </c>

</xml_diff>